<commit_message>
fix description of mehods lab2
</commit_message>
<xml_diff>
--- a/lab2/lab2_results.xlsx
+++ b/lab2/lab2_results.xlsx
@@ -461,13 +461,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5834324217514348</v>
+        <v>1.240874295700121</v>
       </c>
       <c r="C3" t="n">
-        <v>0.974661415002176</v>
+        <v>0.9676903269375425</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6464619445991869</v>
+        <v>0.9262671631783286</v>
       </c>
     </row>
     <row r="4">
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.619848588282323</v>
+        <v>6.103355425606415</v>
       </c>
       <c r="C5" t="n">
-        <v>19.66565340216674</v>
+        <v>20.0138924463398</v>
       </c>
       <c r="D5" t="n">
-        <v>60.48439032645933</v>
+        <v>61.25608461685</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22.56783535494207</v>
+        <v>15.71438568301618</v>
       </c>
       <c r="C8" t="n">
-        <v>209.1012679401471</v>
+        <v>126.7731092634314</v>
       </c>
       <c r="D8" t="n">
-        <v>2402.744458334816</v>
+        <v>2174.868861313473</v>
       </c>
     </row>
     <row r="9">
@@ -558,7 +558,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>H0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>158.3977494298843</v>
+        <v>118.3031466402939</v>
       </c>
       <c r="C10" t="n">
-        <v>1689.050518962632</v>
+        <v>3936.864099980687</v>
       </c>
       <c r="D10" t="n">
-        <v>26594.55755251158</v>
+        <v>31766.96556149196</v>
       </c>
     </row>
     <row r="11">
@@ -627,13 +627,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C13" t="n">
-        <v>684</v>
+        <v>642</v>
       </c>
       <c r="D13" t="n">
-        <v>6810</v>
+        <v>6782</v>
       </c>
     </row>
     <row r="14">
@@ -681,13 +681,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C16" t="n">
-        <v>767</v>
+        <v>744</v>
       </c>
       <c r="D16" t="n">
-        <v>7599</v>
+        <v>7535</v>
       </c>
     </row>
     <row r="17">
@@ -745,13 +745,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.04100000000000004</v>
+        <v>0.04199999999999998</v>
       </c>
       <c r="C20" t="n">
-        <v>0.008400000000000074</v>
+        <v>0.01689999999999992</v>
       </c>
       <c r="D20" t="n">
-        <v>0.003380000000000022</v>
+        <v>0.004319999999999991</v>
       </c>
     </row>
     <row r="21">
@@ -809,13 +809,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1140000000000001</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1043000000000001</v>
+        <v>0.1073000000000001</v>
       </c>
       <c r="D24" t="n">
-        <v>0.09898000000000007</v>
+        <v>0.09263999999999994</v>
       </c>
     </row>
     <row r="25">

</xml_diff>